<commit_message>
finally solve the callback problem
</commit_message>
<xml_diff>
--- a/server/files/week-report.xlsx
+++ b/server/files/week-report.xlsx
@@ -400,16 +400,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <v>greag</v>
+        <v>Debug Nodejs</v>
       </c>
       <c r="B2" t="str">
-        <v>ga</v>
+        <v>4h</v>
       </c>
       <c r="C2" t="str">
-        <v>w</v>
+        <v>Bowen</v>
       </c>
       <c r="D2" t="str">
-        <v>gt</v>
+        <v>99%</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a new line shortcuts
</commit_message>
<xml_diff>
--- a/server/files/week-report.xlsx
+++ b/server/files/week-report.xlsx
@@ -400,16 +400,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <v>Debug Nodejs</v>
+        <v>dq`</v>
       </c>
       <c r="B2" t="str">
-        <v>4h</v>
+        <v>fdawd</v>
       </c>
       <c r="C2" t="str">
-        <v>Bowen</v>
+        <v>fqw</v>
       </c>
       <c r="D2" t="str">
-        <v>99%</v>
+        <v>fqw</v>
       </c>
     </row>
   </sheetData>

</xml_diff>